<commit_message>
Ajout JDV tableaux mapping 3fffaa3a34ee230cdf7665178d2f7cc924f0f907
</commit_message>
<xml_diff>
--- a/ig/amelioration-mapping/StructureDefinition-RORPractitionerRoleName.xlsx
+++ b/ig/amelioration-mapping/StructureDefinition-RORPractitionerRoleName.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-24T16:02:26+00:00</t>
+    <t>2024-02-06T12:55:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -318,7 +318,7 @@
     <t>exerciseTitle</t>
   </si>
   <si>
-    <t>civiliteExercice</t>
+    <t>civiliteExercice : JDV-J208-CiviliteExercice-ROR</t>
   </si>
   <si>
     <t>Extension.extension:exerciseTitle.id</t>

</xml_diff>